<commit_message>
Added update to Gannt Chart, changes in implementation order
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Year 3\Comp3000\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woody\Official\COMP3000\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B37C415-C493-49E9-BE4B-3E9B32EA838B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14CB7C7-E57A-451E-91BA-E9F094ECCB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D6CA7327-8391-4ADC-A46A-1094BD6B68B5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{D6CA7327-8391-4ADC-A46A-1094BD6B68B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -75,12 +75,6 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Further Improvements</t>
-  </si>
-  <si>
-    <t>Potential Further Exercises and Refinement</t>
-  </si>
-  <si>
     <t>Quiz Research and Creation</t>
   </si>
   <si>
@@ -118,6 +112,12 @@
   </si>
   <si>
     <t>Excerise 4 - Recognizing Insider Threats</t>
+  </si>
+  <si>
+    <t>Improvements from Testing</t>
+  </si>
+  <si>
+    <t>Phishing Malware Simulation</t>
   </si>
 </sst>
 </file>
@@ -198,7 +198,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -329,25 +329,25 @@
                   <c:v>Exercise 2 - Password Strength Tester </c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Greeting/ Task information </c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Progress Tracker</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Quiz Research and Creation</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Quizzes Implementation </c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Phishing Malware Simulation</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Exercise 3 - Safe Web Browsing &amp; Malware Downloads</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16">
                   <c:v>Excerise 4 - Recognizing Insider Threats</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Potential Further Exercises and Refinement</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Greeting/ Task information </c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Progress Tracker</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Quiz Research and Creation</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Quizzes Implementation </c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>Score Implementation</c:v>
@@ -356,7 +356,7 @@
                   <c:v>Testing</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Further Improvements</c:v>
+                  <c:v>Improvements from Testing</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Poster and Description</c:v>
@@ -508,25 +508,25 @@
                   <c:v>Exercise 2 - Password Strength Tester </c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Greeting/ Task information </c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Progress Tracker</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Quiz Research and Creation</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Quizzes Implementation </c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Phishing Malware Simulation</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Exercise 3 - Safe Web Browsing &amp; Malware Downloads</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16">
                   <c:v>Excerise 4 - Recognizing Insider Threats</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Potential Further Exercises and Refinement</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Greeting/ Task information </c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Progress Tracker</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Quiz Research and Creation</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Quizzes Implementation </c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>Score Implementation</c:v>
@@ -535,7 +535,7 @@
                   <c:v>Testing</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Further Improvements</c:v>
+                  <c:v>Improvements from Testing</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>Poster and Description</c:v>
@@ -1347,7 +1347,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3EF4FB33-4389-4F14-AF7E-1A9E25D13790}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="120" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1706,8 +1706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5007213-0D92-410E-AC54-80C5C3AB5883}">
   <dimension ref="A3:N27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,16 +1746,16 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1857,8 +1857,8 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
+      <c r="A12" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B12" s="2">
         <v>45608</v>
@@ -1871,8 +1871,8 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
+      <c r="A13" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B13" s="2">
         <v>45618</v>
@@ -1885,8 +1885,8 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
+      <c r="A14" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B14" s="2">
         <v>45628</v>
@@ -1899,8 +1899,8 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
+      <c r="A15" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B15" s="2">
         <v>45635</v>
@@ -1914,7 +1914,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B16" s="2">
         <v>45642</v>
@@ -1928,7 +1928,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2">
         <v>45649</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2">
         <v>45667</v>
@@ -1956,7 +1956,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2">
         <v>45677</v>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B20" s="2">
         <v>45684</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2">
         <v>45684</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2">
         <v>45702</v>
@@ -2040,7 +2040,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25" s="2">
         <v>45730</v>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B26" s="2">
         <v>45737</v>
@@ -2066,12 +2066,12 @@
         <v>38</v>
       </c>
       <c r="M26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>